<commit_message>
Update to chip status. Added LAL calibration data.
</commit_message>
<xml_diff>
--- a/ChipStatus.xlsx
+++ b/ChipStatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="57">
   <si>
     <t>chip OK, old criterion</t>
   </si>
@@ -93,9 +93,6 @@
     <t>low gain (2 runs)</t>
   </si>
   <si>
-    <t>one channel at half</t>
-  </si>
-  <si>
     <t>one channel at half (1.5 runs)</t>
   </si>
   <si>
@@ -142,13 +139,61 @@
   </si>
   <si>
     <t>rejected by Promex</t>
+  </si>
+  <si>
+    <t>one channel at half, valid at LAL</t>
+  </si>
+  <si>
+    <t>gains too low</t>
+  </si>
+  <si>
+    <t>low gain</t>
+  </si>
+  <si>
+    <t>low gain noise</t>
+  </si>
+  <si>
+    <t>channel on test 1, low gain (2 tests)</t>
+  </si>
+  <si>
+    <t>low gain (2 tests)</t>
+  </si>
+  <si>
+    <t>no signal, 2 tests</t>
+  </si>
+  <si>
+    <t>one channel at half (1 run)</t>
+  </si>
+  <si>
+    <t>gain noise</t>
+  </si>
+  <si>
+    <t>gain linearity</t>
+  </si>
+  <si>
+    <t>linearity</t>
+  </si>
+  <si>
+    <t>linearity, noise</t>
+  </si>
+  <si>
+    <t>New PostScreening Test  incidents</t>
+  </si>
+  <si>
+    <t>New PostScreening Test result</t>
+  </si>
+  <si>
+    <t>noise 1,2,3</t>
+  </si>
+  <si>
+    <t>rejected by Promex, power consumption</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +201,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +266,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,12 +309,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,11 +636,13 @@
     <col min="2" max="2" width="11.42578125" style="2"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -554,8 +664,14 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -581,270 +697,508 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>102</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>103</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>104</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>105</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>106</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>107</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F8" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>108</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>110</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>112</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>113</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>114</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>115</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>116</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <v>117</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>120</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>121</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>122</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>123</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>124</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D25" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
         <v>126</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>127</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
         <v>128</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D29" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="F29" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
         <v>129</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
         <v>130</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>131</v>
       </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D32" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
         <v>132</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>134</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
         <v>135</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
@@ -852,37 +1206,73 @@
       <c r="D36" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>136</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>137</v>
       </c>
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
         <v>138</v>
       </c>
+      <c r="B39" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
         <v>139</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
@@ -890,179 +1280,308 @@
       <c r="D40" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
         <v>140</v>
       </c>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D41" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>141</v>
       </c>
       <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>142</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <v>143</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>142</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>143</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <v>144</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>144</v>
-      </c>
-      <c r="C45" t="s">
-        <v>27</v>
-      </c>
       <c r="D45" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
         <v>146</v>
       </c>
+      <c r="B47" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D47" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F47" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>148</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>149</v>
       </c>
+      <c r="B50" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="E50" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>150</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>150</v>
-      </c>
-      <c r="C51" t="s">
-        <v>33</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>151</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="C52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
         <v>152</v>
       </c>
+      <c r="B53" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="E53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
         <v>153</v>
       </c>
+      <c r="B54" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C54" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
         <v>155</v>
       </c>
+      <c r="B56" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D56" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F56" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>157</v>
       </c>
+      <c r="B58" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="C58" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>158</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="C59" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="13">
         <v>159</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -1078,13 +1597,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>160</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="13">
         <v>161</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -1097,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>162</v>
       </c>
@@ -1107,28 +1632,31 @@
       <c r="C63" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G63" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>201</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>202</v>
       </c>
+      <c r="B65" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D65" s="3" t="s">
         <v>1</v>
       </c>
@@ -1136,10 +1664,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>203</v>
       </c>
+      <c r="B66" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C66" t="s">
         <v>19</v>
       </c>
@@ -1150,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>204</v>
       </c>
@@ -1166,14 +1697,17 @@
       <c r="E67" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>205</v>
       </c>
+      <c r="B68" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D68" s="3" t="s">
         <v>1</v>
       </c>
@@ -1181,10 +1715,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>206</v>
       </c>
+      <c r="B69" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C69" t="s">
         <v>21</v>
       </c>
@@ -1195,10 +1732,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>207</v>
       </c>
+      <c r="B70" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D70" s="3" t="s">
         <v>1</v>
       </c>
@@ -1206,10 +1746,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>208</v>
       </c>
+      <c r="B71" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D71" s="3" t="s">
         <v>1</v>
       </c>
@@ -1217,140 +1760,248 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>209</v>
       </c>
+      <c r="B72" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D72" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>210</v>
       </c>
+      <c r="B73" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C73" t="s">
         <v>15</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>211</v>
       </c>
+      <c r="B74" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D74" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>212</v>
       </c>
+      <c r="B75" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D75" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>213</v>
       </c>
+      <c r="B76" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D76" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J76" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>214</v>
       </c>
+      <c r="B77" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D77" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>215</v>
       </c>
+      <c r="B78" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D78" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>216</v>
       </c>
+      <c r="B79" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D79" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>217</v>
       </c>
+      <c r="B80" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D80" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F80" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>218</v>
       </c>
+      <c r="B81" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D81" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F81" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>219</v>
       </c>
+      <c r="B82" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D82" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>42</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J82" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>220</v>
       </c>
+      <c r="B83" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D83" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>24</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J83" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>221</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>222</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D85" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>223</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>224</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D87" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>225</v>
       </c>
+      <c r="B88" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C88" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>226</v>
       </c>
@@ -1360,16 +2011,19 @@
       <c r="E89" t="s">
         <v>15</v>
       </c>
-      <c r="F89" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F89" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>227</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D90" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>228</v>
       </c>
@@ -1382,17 +2036,17 @@
       <c r="E91" t="s">
         <v>24</v>
       </c>
-      <c r="F91" s="4" t="s">
+      <c r="F91" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G91" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H91" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>229</v>
       </c>
@@ -1403,28 +2057,28 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H92" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>231</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>233</v>
       </c>

</xml_diff>

<commit_message>
Added SCP VIs and transfer queue (to be tested).
</commit_message>
<xml_diff>
--- a/ChipStatus.xlsx
+++ b/ChipStatus.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="74">
   <si>
     <t>chip OK, old criterion</t>
   </si>
@@ -210,7 +211,34 @@
     <t>OK on soldered board</t>
   </si>
   <si>
-    <t>missing channel (3 tests)</t>
+    <t>rejected by Promex, bad channel (3 tests)</t>
+  </si>
+  <si>
+    <t>same bad channel</t>
+  </si>
+  <si>
+    <t>missing channel (4 tests)</t>
+  </si>
+  <si>
+    <t>rejected by Promex, bad channel</t>
+  </si>
+  <si>
+    <t>rejected by Promex, no signal</t>
+  </si>
+  <si>
+    <t>same no signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SLAC for board</t>
+  </si>
+  <si>
+    <t>SLAC for CSAM</t>
+  </si>
+  <si>
+    <t>CENBG</t>
   </si>
 </sst>
 </file>
@@ -274,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +339,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -339,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,8 +395,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +747,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="15">
         <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -879,7 +921,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="18">
         <v>111</v>
       </c>
       <c r="C12" t="s">
@@ -896,7 +938,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="18">
         <v>112</v>
       </c>
       <c r="C13" t="s">
@@ -1004,7 +1046,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="18">
         <v>118</v>
       </c>
       <c r="C19" t="s">
@@ -1013,7 +1055,7 @@
       <c r="D19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1063,7 +1105,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="18">
         <v>122</v>
       </c>
       <c r="C23" t="s">
@@ -1072,7 +1114,7 @@
       <c r="D23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1117,7 +1159,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="18">
         <v>125</v>
       </c>
       <c r="C26" t="s">
@@ -1126,7 +1168,7 @@
       <c r="D26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1469,11 +1511,20 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="18">
         <v>145</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>64</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -1559,16 +1610,16 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="18">
         <v>151</v>
       </c>
       <c r="C52" t="s">
         <v>40</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1619,13 +1670,19 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="18">
         <v>154</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1678,13 +1735,19 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="18">
         <v>158</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" t="s">
+        <v>69</v>
+      </c>
+      <c r="F59" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1734,7 +1797,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="15">
         <v>162</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -1766,10 +1829,12 @@
       <c r="D64" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F64" s="8"/>
+      <c r="F64" s="8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="13">
+      <c r="A65" s="18">
         <v>164</v>
       </c>
       <c r="C65" t="s">
@@ -1784,10 +1849,10 @@
       <c r="A66" s="14">
         <v>200</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F66" s="16" t="s">
+      <c r="F66" s="17" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1798,7 +1863,7 @@
       <c r="D67" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F67" s="16" t="s">
+      <c r="F67" s="17" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2102,7 +2167,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="15">
         <v>221</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -2116,7 +2181,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88">
+      <c r="A88" s="15">
         <v>222</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -2128,12 +2193,15 @@
       <c r="F88" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="G88" t="s">
+        <v>35</v>
+      </c>
       <c r="I88" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="A89" s="15">
         <v>223</v>
       </c>
       <c r="C89" t="s">
@@ -2147,11 +2215,14 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="A90" s="15">
         <v>224</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="G90" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -2172,7 +2243,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92">
+      <c r="A92" s="15">
         <v>226</v>
       </c>
       <c r="D92" s="3" t="s">
@@ -2189,7 +2260,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="A93" s="15">
         <v>227</v>
       </c>
       <c r="D93" s="3" t="s">
@@ -2290,7 +2361,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="A100" s="15">
         <v>234</v>
       </c>
       <c r="C100" t="s">
@@ -2304,6 +2375,21 @@
       </c>
       <c r="F100" s="9" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated chip status list.
</commit_message>
<xml_diff>
--- a/ChipStatus.xlsx
+++ b/ChipStatus.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="76">
   <si>
     <t>chip OK, old criterion</t>
   </si>
@@ -229,9 +228,6 @@
     <t>same no signal</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>SLAC for board</t>
   </si>
   <si>
@@ -239,6 +235,15 @@
   </si>
   <si>
     <t>CENBG</t>
+  </si>
+  <si>
+    <t>OK including TEMP</t>
+  </si>
+  <si>
+    <t>Soldered: shorts to ground, test unsoldered</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -302,7 +307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +356,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -381,7 +392,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -399,6 +409,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,35 +713,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G1" t="s">
@@ -742,27 +753,27 @@
       <c r="I1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="14">
         <v>101</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
@@ -773,54 +784,54 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>102</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>103</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>104</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="11" t="s">
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -828,64 +839,67 @@
       <c r="A6">
         <v>105</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>106</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>107</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>108</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -893,13 +907,16 @@
       <c r="A10">
         <v>109</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -907,73 +924,79 @@
       <c r="A11">
         <v>110</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <v>111</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <v>112</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>113</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="11" t="s">
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -981,10 +1004,13 @@
       <c r="A15">
         <v>114</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -992,25 +1018,25 @@
       <c r="A16">
         <v>115</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
+      <c r="B16" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I16" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1018,44 +1044,50 @@
       <c r="A17">
         <v>116</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="12">
         <v>117</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="D18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="A19" s="17">
         <v>118</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="9" t="s">
+      <c r="D19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1063,30 +1095,33 @@
       <c r="A20">
         <v>119</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="4" t="s">
+      <c r="D20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="12">
         <v>120</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1094,50 +1129,56 @@
       <c r="A22">
         <v>121</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="D22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
+      <c r="A23" s="17">
         <v>122</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="9" t="s">
+      <c r="D23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="A24" s="12">
         <v>123</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="11" t="s">
+      <c r="F24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1145,44 +1186,47 @@
       <c r="A25">
         <v>124</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J25" s="11" t="s">
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="A26" s="17">
         <v>125</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C26" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="9" t="s">
+      <c r="D26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="12">
         <v>126</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H27" t="s">
@@ -1193,73 +1237,76 @@
       <c r="A28">
         <v>127</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C28" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="4" t="s">
+      <c r="D28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="A29" s="12">
         <v>128</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>129</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="11" t="s">
+      <c r="F30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+      <c r="A31" s="12">
         <v>130</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="11" t="s">
+      <c r="F31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1267,30 +1314,33 @@
       <c r="A32">
         <v>131</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E32" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="11" t="s">
+      <c r="F32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
+      <c r="A33" s="12">
         <v>132</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1298,13 +1348,16 @@
       <c r="A34">
         <v>133</v>
       </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C34" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="4" t="s">
+      <c r="D34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1312,30 +1365,33 @@
       <c r="A35">
         <v>134</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C35" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="4" t="s">
+      <c r="D35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="A36" s="12">
         <v>135</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="4" t="s">
+      <c r="D36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1343,13 +1399,16 @@
       <c r="A37">
         <v>136</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C37" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="D37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1357,91 +1416,91 @@
       <c r="A38">
         <v>137</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G38" t="s">
         <v>63</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="J38" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+      <c r="A39" s="12">
         <v>138</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="11" t="s">
+      <c r="F39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="A40" s="12">
         <v>139</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
         <v>49</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="11" t="s">
+      <c r="F40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+      <c r="A41" s="12">
         <v>140</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
         <v>50</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="11" t="s">
+      <c r="F41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1452,92 +1511,99 @@
       <c r="C42" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+      <c r="A43" s="12">
         <v>142</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="13">
+      <c r="A44" s="12">
         <v>143</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
       </c>
+      <c r="D44" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E44" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+      <c r="A45" s="12">
         <v>144</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E45" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="11" t="s">
+      <c r="F45" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="18">
+      <c r="A46" s="17">
         <v>145</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C46" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E46" t="s">
         <v>65</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="13">
+      <c r="A47" s="12">
         <v>146</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" s="4" t="s">
+      <c r="B47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1548,9 +1614,10 @@
       <c r="C48" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -1559,144 +1626,154 @@
       <c r="C49" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="18"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>149</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E50" t="s">
         <v>43</v>
       </c>
-      <c r="F50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J50" s="11" t="s">
+      <c r="F50" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="13">
+      <c r="A51" s="12">
         <v>150</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E51" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J51" s="11" t="s">
+      <c r="F51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
+      <c r="A52" s="17">
         <v>151</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C52" t="s">
         <v>40</v>
       </c>
+      <c r="D52" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E52" t="s">
         <v>66</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="13">
+      <c r="A53" s="12">
         <v>152</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E53" t="s">
         <v>46</v>
       </c>
-      <c r="F53" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53" s="11" t="s">
+      <c r="F53" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="13">
+      <c r="A54" s="12">
         <v>153</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C54" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E54" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J54" s="11" t="s">
+      <c r="F54" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="18">
+      <c r="A55" s="17">
         <v>154</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C55" t="s">
         <v>67</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E55" t="s">
         <v>65</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="13">
+      <c r="A56" s="12">
         <v>155</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" s="4" t="s">
+      <c r="B56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1704,13 +1781,16 @@
       <c r="A57">
         <v>156</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C57" t="s">
         <v>40</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F57" s="4" t="s">
+      <c r="D57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1718,53 +1798,56 @@
       <c r="A58">
         <v>157</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C58" t="s">
         <v>34</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E58" t="s">
         <v>47</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="18">
+      <c r="A59" s="17">
         <v>158</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C59" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E59" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="13">
+      <c r="A60" s="12">
         <v>159</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="D60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1772,47 +1855,50 @@
       <c r="A61">
         <v>160</v>
       </c>
+      <c r="B61" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C61" t="s">
         <v>40</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="D61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="13">
+      <c r="A62" s="12">
         <v>161</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="B62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="15">
+      <c r="A63" s="14">
         <v>162</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F63" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G63" t="s">
@@ -1820,39 +1906,48 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>163</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C64" t="s">
         <v>40</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>70</v>
+      <c r="D64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="18">
+      <c r="A65" s="17">
         <v>164</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C65" t="s">
         <v>40</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F65" s="8"/>
+      <c r="D65" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="14">
+      <c r="A66" s="13">
         <v>200</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="B66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F66" s="17" t="s">
+      <c r="F66" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1860,41 +1955,44 @@
       <c r="A67">
         <v>201</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="B67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F67" s="17" t="s">
+      <c r="F67" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="13">
+      <c r="A68" s="12">
         <v>202</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F68" s="4" t="s">
+      <c r="B68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="13">
+      <c r="A69" s="12">
         <v>203</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C69" t="s">
         <v>19</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F69" s="4" t="s">
+      <c r="D69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1902,295 +2000,301 @@
       <c r="A70">
         <v>204</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C70" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F70" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="H70" t="s">
+        <v>74</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
+      <c r="A71" s="12">
         <v>205</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F71" s="4" t="s">
+      <c r="B71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="13">
+      <c r="A72" s="12">
         <v>206</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C72" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F72" s="4" t="s">
+      <c r="D72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="13">
+      <c r="A73" s="12">
         <v>207</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F73" s="4" t="s">
+      <c r="B73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="13">
+      <c r="A74" s="12">
         <v>208</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F74" s="4" t="s">
+      <c r="B74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="13">
+      <c r="A75" s="12">
         <v>209</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F75" s="4" t="s">
+      <c r="B75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="13">
+      <c r="A76" s="12">
         <v>210</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C76" t="s">
         <v>15</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F76" s="4" t="s">
+      <c r="D76" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="13">
+      <c r="A77" s="12">
         <v>211</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F77" s="4" t="s">
+      <c r="B77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="13">
+      <c r="A78" s="12">
         <v>212</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F78" s="4" t="s">
+      <c r="B78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="13">
+      <c r="A79" s="12">
         <v>213</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="3" t="s">
+      <c r="B79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
       </c>
-      <c r="F79" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J79" s="11" t="s">
+      <c r="F79" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J79" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="13">
+      <c r="A80" s="12">
         <v>214</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F80" s="4" t="s">
+      <c r="B80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="13">
+      <c r="A81" s="12">
         <v>215</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F81" s="4" t="s">
+      <c r="B81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="13">
+      <c r="A82" s="12">
         <v>216</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F82" s="4" t="s">
+      <c r="B82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="13">
+      <c r="A83" s="12">
         <v>217</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F83" s="4" t="s">
+      <c r="B83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="13">
+      <c r="A84" s="12">
         <v>218</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F84" s="4" t="s">
+      <c r="B84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="13">
+      <c r="A85" s="12">
         <v>219</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="3" t="s">
+      <c r="B85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E85" t="s">
         <v>42</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J85" s="11" t="s">
+      <c r="F85" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J85" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="13">
+      <c r="A86" s="12">
         <v>220</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" s="3" t="s">
+      <c r="B86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E86" t="s">
         <v>24</v>
       </c>
-      <c r="F86" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J86" s="11" t="s">
+      <c r="F86" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="15">
+      <c r="A87" s="14">
         <v>221</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F87" s="4" t="s">
+      <c r="B87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="15">
+      <c r="A88" s="14">
         <v>222</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F88" s="8" t="s">
+      <c r="D88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G88" t="s">
@@ -2201,24 +2305,30 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="15">
+      <c r="A89" s="14">
         <v>223</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C89" t="s">
         <v>15</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F89" s="4" t="s">
+      <c r="D89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="15">
+      <c r="A90" s="14">
         <v>224</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="B90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G90" t="s">
@@ -2226,47 +2336,53 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="13">
+      <c r="A91" s="12">
         <v>225</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C91" t="s">
         <v>15</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F91" s="4" t="s">
+      <c r="D91" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="15">
+      <c r="A92" s="14">
         <v>226</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="B92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="11" t="s">
+      <c r="F92" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J92" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="15">
+      <c r="A93" s="14">
         <v>227</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F93" s="4" t="s">
+      <c r="B93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2274,19 +2390,19 @@
       <c r="A94">
         <v>228</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C94" t="s">
         <v>17</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E94" t="s">
         <v>24</v>
       </c>
-      <c r="F94" s="8" t="s">
+      <c r="F94" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G94" t="s">
@@ -2300,13 +2416,13 @@
       <c r="A95">
         <v>229</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F95" s="4" t="s">
+      <c r="D95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G95" t="s">
@@ -2320,10 +2436,13 @@
       <c r="A96">
         <v>230</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="B96" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="F96" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2331,10 +2450,13 @@
       <c r="A97">
         <v>231</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="B97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F97" s="4" t="s">
+      <c r="F97" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2342,10 +2464,13 @@
       <c r="A98">
         <v>232</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="B98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F98" s="4" t="s">
+      <c r="F98" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2353,43 +2478,49 @@
       <c r="A99">
         <v>233</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="B99" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F99" s="4" t="s">
+      <c r="F99" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="15">
+      <c r="A100" s="14">
         <v>234</v>
+      </c>
+      <c r="B100" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C100" t="s">
         <v>57</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E100" t="s">
         <v>57</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F100" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
+      <c r="A104" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="15" t="s">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="18" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update of chip status.
</commit_message>
<xml_diff>
--- a/ChipStatus.xlsx
+++ b/ChipStatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="77">
   <si>
     <t>chip OK, old criterion</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Extra screening 24h+reflow1 OK, OK 2+3</t>
   </si>
 </sst>
 </file>
@@ -713,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,17 +893,20 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2231,11 +2237,11 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="12">
+      <c r="A85" s="13">
         <v>219</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>1</v>
@@ -2245,6 +2251,9 @@
       </c>
       <c r="F85" s="7" t="s">
         <v>16</v>
+      </c>
+      <c r="G85" t="s">
+        <v>76</v>
       </c>
       <c r="J85" s="10" t="s">
         <v>1</v>
@@ -2329,6 +2338,9 @@
         <v>7</v>
       </c>
       <c r="D90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G90" t="s">

</xml_diff>

<commit_message>
LAL calibration, update to analysis.
</commit_message>
<xml_diff>
--- a/ChipStatus.xlsx
+++ b/ChipStatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="80">
   <si>
     <t>chip OK, old criterion</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>Extra screening 24h+reflow1 OK, OK 2+3</t>
+  </si>
+  <si>
+    <t>Extra screening 48h+reflow1+2+3 OK</t>
+  </si>
+  <si>
+    <t>Extra screening 72h+reflow1+2+3 OK</t>
+  </si>
+  <si>
+    <t>Distrel</t>
   </si>
 </sst>
 </file>
@@ -716,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,11 +1073,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>117</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
@@ -1078,6 +1087,9 @@
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1617,6 +1629,9 @@
       <c r="A48">
         <v>147</v>
       </c>
+      <c r="B48" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C48" t="s">
         <v>28</v>
       </c>
@@ -1629,6 +1644,9 @@
       <c r="A49">
         <v>148</v>
       </c>
+      <c r="B49" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C49" t="s">
         <v>29</v>
       </c>
@@ -1841,11 +1859,11 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="12">
+      <c r="A60" s="13">
         <v>159</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -1855,6 +1873,9 @@
       </c>
       <c r="F60" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2260,11 +2281,11 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="12">
+      <c r="A86" s="13">
         <v>220</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>1</v>
@@ -2274,6 +2295,9 @@
       </c>
       <c r="F86" s="7" t="s">
         <v>16</v>
+      </c>
+      <c r="G86" t="s">
+        <v>77</v>
       </c>
       <c r="J86" s="10" t="s">
         <v>1</v>
@@ -2314,11 +2338,11 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="14">
+      <c r="A89" s="13">
         <v>223</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C89" t="s">
         <v>15</v>
@@ -2328,6 +2352,9 @@
       </c>
       <c r="F89" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="G89" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Production version for top VI.
</commit_message>
<xml_diff>
--- a/ChipStatus.xlsx
+++ b/ChipStatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="82">
   <si>
     <t>chip OK, old criterion</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>IPNL</t>
+  </si>
+  <si>
+    <t>BNL</t>
   </si>
 </sst>
 </file>
@@ -322,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +380,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -405,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -425,6 +434,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1029,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="19">
         <v>114</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1332,7 +1342,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="19">
         <v>131</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1968,7 +1978,7 @@
       <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="13">
+      <c r="A66" s="19">
         <v>200</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1982,7 +1992,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="19">
         <v>201</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2475,7 +2485,7 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="A96" s="19">
         <v>230</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2489,7 +2499,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="A97" s="19">
         <v>231</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -2503,7 +2513,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98">
+      <c r="A98" s="19">
         <v>232</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -2563,6 +2573,11 @@
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>